<commit_message>
Update VERA - Referentiedata - 2022-02-18.xlsx
Huuropzegging status
</commit_message>
<xml_diff>
--- a/Referentiedata/VERA - Referentiedata - 2022-02-18.xlsx
+++ b/Referentiedata/VERA - Referentiedata - 2022-02-18.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VERA\VERA-Standaard\Referentiedata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C49012-71A2-452F-A155-22E79D053AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3453AB89-9C54-43E9-ADE9-2229CDC26FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5469" yWindow="1500" windowWidth="18720" windowHeight="11597" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6309" yWindow="4260" windowWidth="21514" windowHeight="11597" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VERA referentiedata" sheetId="14" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8093" uniqueCount="4144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8111" uniqueCount="4145">
   <si>
     <t>Referentiedatasoort</t>
   </si>
@@ -12564,6 +12564,9 @@
   </si>
   <si>
     <t>Een buitenlands adres</t>
+  </si>
+  <si>
+    <t>HUUROPZEGGINGSTATUS</t>
   </si>
 </sst>
 </file>
@@ -13310,8 +13313,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}" name="Tabel1" displayName="Tabel1" ref="A1:K1283" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:K1283" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}" name="Tabel1" displayName="Tabel1" ref="A1:K1289" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:K1289" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K1283">
     <sortCondition ref="A1:A1283"/>
   </sortState>
@@ -13686,11 +13689,11 @@
   <sheetPr codeName="Blad1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L1283"/>
+  <dimension ref="A1:L1289"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1295" sqref="B1295"/>
+      <pane ySplit="1" topLeftCell="A1277" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1284" sqref="A1284:A1289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -42563,6 +42566,120 @@
       </c>
       <c r="J1283" s="13"/>
       <c r="K1283" s="13"/>
+    </row>
+    <row r="1284" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1284" s="10" t="s">
+        <v>4144</v>
+      </c>
+      <c r="B1284" s="10"/>
+      <c r="C1284" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1284" s="11" t="s">
+        <v>3842</v>
+      </c>
+      <c r="E1284" s="11"/>
+      <c r="F1284" s="11"/>
+      <c r="G1284" s="11"/>
+      <c r="H1284" s="10"/>
+      <c r="I1284" s="10"/>
+      <c r="J1284" s="10"/>
+      <c r="K1284" s="10"/>
+    </row>
+    <row r="1285" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1285" s="10" t="s">
+        <v>4144</v>
+      </c>
+      <c r="B1285" s="10"/>
+      <c r="C1285" s="10" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D1285" s="11" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E1285" s="11"/>
+      <c r="F1285" s="11"/>
+      <c r="G1285" s="11"/>
+      <c r="H1285" s="10"/>
+      <c r="I1285" s="10"/>
+      <c r="J1285" s="10"/>
+      <c r="K1285" s="10"/>
+    </row>
+    <row r="1286" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1286" s="10" t="s">
+        <v>4144</v>
+      </c>
+      <c r="B1286" s="10"/>
+      <c r="C1286" s="10" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D1286" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1286" s="11"/>
+      <c r="F1286" s="11"/>
+      <c r="G1286" s="11"/>
+      <c r="H1286" s="10"/>
+      <c r="I1286" s="10"/>
+      <c r="J1286" s="10"/>
+      <c r="K1286" s="10"/>
+    </row>
+    <row r="1287" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1287" s="10" t="s">
+        <v>4144</v>
+      </c>
+      <c r="B1287" s="10"/>
+      <c r="C1287" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1287" s="11" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E1287" s="11"/>
+      <c r="F1287" s="11"/>
+      <c r="G1287" s="11"/>
+      <c r="H1287" s="10"/>
+      <c r="I1287" s="10"/>
+      <c r="J1287" s="10"/>
+      <c r="K1287" s="10"/>
+    </row>
+    <row r="1288" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1288" s="10" t="s">
+        <v>4144</v>
+      </c>
+      <c r="B1288" s="10"/>
+      <c r="C1288" s="10" t="s">
+        <v>521</v>
+      </c>
+      <c r="D1288" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1288" s="11"/>
+      <c r="F1288" s="11"/>
+      <c r="G1288" s="11"/>
+      <c r="H1288" s="10"/>
+      <c r="I1288" s="10"/>
+      <c r="J1288" s="10"/>
+      <c r="K1288" s="10"/>
+    </row>
+    <row r="1289" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1289" s="10" t="s">
+        <v>4144</v>
+      </c>
+      <c r="B1289" s="10"/>
+      <c r="C1289" s="10" t="s">
+        <v>1481</v>
+      </c>
+      <c r="D1289" s="11" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E1289" s="11"/>
+      <c r="F1289" s="11"/>
+      <c r="G1289" s="11"/>
+      <c r="H1289" s="10"/>
+      <c r="I1289" s="10"/>
+      <c r="J1289" s="10"/>
+      <c r="K1289" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
@@ -49011,18 +49128,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -49045,18 +49162,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6EB239C-D482-4083-A20F-2310AB45B47F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E3AA29B-E85A-4662-AF70-E41EEBB4502A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6EB239C-D482-4083-A20F-2310AB45B47F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>